<commit_message>
Kateryna - commit 11
</commit_message>
<xml_diff>
--- a/Personal_info_data.xlsx
+++ b/Personal_info_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kater\IdeaProjects\bdd-sprint3-framework\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="218">
   <si>
     <t>bFirst_Name</t>
   </si>
@@ -668,12 +668,19 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1025,13 +1032,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.08203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.08203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.1640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1088,6 +1095,9 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
+      <c r="I2" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1114,6 +1124,9 @@
       <c r="H3" t="s">
         <v>19</v>
       </c>
+      <c r="I3" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1140,6 +1153,9 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
+      <c r="I4" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1166,6 +1182,9 @@
       <c r="H5" t="s">
         <v>33</v>
       </c>
+      <c r="I5" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1192,6 +1211,9 @@
       <c r="H6" t="s">
         <v>40</v>
       </c>
+      <c r="I6" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1217,6 +1239,9 @@
       </c>
       <c r="H7" t="s">
         <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>